<commit_message>
Cambios debido a cambios en DB
Cambie el excel, la lista de paises en la pagina y un detallito en el excel
</commit_message>
<xml_diff>
--- a/Web/Excel/Ejemplo.xlsx
+++ b/Web/Excel/Ejemplo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edy\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edy\Documents\GitHub\Proyecto2\Web\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -406,7 +406,7 @@
     <t>GTM</t>
   </si>
   <si>
-    <t>Mex</t>
+    <t>MEX</t>
   </si>
 </sst>
 </file>
@@ -979,7 +979,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>